<commit_message>
// Project : -RES Power trading -ID Trading
STEP 1 :
-Connexion to RTE ENTSOE APIs
-Building automatic reports - DA auctions
</commit_message>
<xml_diff>
--- a/Data/DA_PriceFR.xlsx
+++ b/Data/DA_PriceFR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CYTech Student\PycharmProjects\Quantitative_Finance\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E276C34F-29A1-4451-847C-7D9E7050B8AF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE1EB869-6D88-4040-87ED-9A4B2932CC0D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -92,7 +92,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -395,10 +395,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C73"/>
+  <dimension ref="A1:C49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="A73" sqref="A73"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -945,270 +945,6 @@
         <v>38.5</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="2">
-        <v>45761</v>
-      </c>
-      <c r="B50">
-        <v>23433.8</v>
-      </c>
-      <c r="C50">
-        <v>39.229999999999997</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="2">
-        <v>45761.041666666657</v>
-      </c>
-      <c r="B51">
-        <v>23721.599999999999</v>
-      </c>
-      <c r="C51">
-        <v>38.159999999999997</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="2">
-        <v>45761.083333333343</v>
-      </c>
-      <c r="B52">
-        <v>24885.4</v>
-      </c>
-      <c r="C52">
-        <v>37.74</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="2">
-        <v>45761.125</v>
-      </c>
-      <c r="B53">
-        <v>26720.400000000001</v>
-      </c>
-      <c r="C53">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="2">
-        <v>45761.166666666657</v>
-      </c>
-      <c r="B54">
-        <v>27088.2</v>
-      </c>
-      <c r="C54">
-        <v>30.01</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="2">
-        <v>45761.208333333343</v>
-      </c>
-      <c r="B55">
-        <v>25703.599999999999</v>
-      </c>
-      <c r="C55">
-        <v>35.01</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="2">
-        <v>45761.25</v>
-      </c>
-      <c r="B56">
-        <v>25638.6</v>
-      </c>
-      <c r="C56">
-        <v>42.5</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="2">
-        <v>45761.291666666657</v>
-      </c>
-      <c r="B57">
-        <v>25631</v>
-      </c>
-      <c r="C57">
-        <v>68.19</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="2">
-        <v>45761.333333333343</v>
-      </c>
-      <c r="B58">
-        <v>26469.4</v>
-      </c>
-      <c r="C58">
-        <v>74.94</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="2">
-        <v>45761.375</v>
-      </c>
-      <c r="B59">
-        <v>25453.200000000001</v>
-      </c>
-      <c r="C59">
-        <v>37.74</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="2">
-        <v>45761.416666666657</v>
-      </c>
-      <c r="B60">
-        <v>29166.400000000001</v>
-      </c>
-      <c r="C60">
-        <v>41.7</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="2">
-        <v>45761.458333333343</v>
-      </c>
-      <c r="B61">
-        <v>32201.599999999999</v>
-      </c>
-      <c r="C61">
-        <v>26.77</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="2">
-        <v>45761.5</v>
-      </c>
-      <c r="B62">
-        <v>34122</v>
-      </c>
-      <c r="C62">
-        <v>52.65</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="2">
-        <v>45761.541666666657</v>
-      </c>
-      <c r="B63">
-        <v>34824.400000000001</v>
-      </c>
-      <c r="C63">
-        <v>23.51</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="2">
-        <v>45761.583333333343</v>
-      </c>
-      <c r="B64">
-        <v>34221.800000000003</v>
-      </c>
-      <c r="C64">
-        <v>10.16</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="2">
-        <v>45761.625</v>
-      </c>
-      <c r="B65">
-        <v>30770.799999999999</v>
-      </c>
-      <c r="C65">
-        <v>20.239999999999998</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="2">
-        <v>45761.666666666657</v>
-      </c>
-      <c r="B66">
-        <v>27411.4</v>
-      </c>
-      <c r="C66">
-        <v>28.12</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="2">
-        <v>45761.708333333343</v>
-      </c>
-      <c r="B67">
-        <v>24996.2</v>
-      </c>
-      <c r="C67">
-        <v>38.46</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="2">
-        <v>45761.75</v>
-      </c>
-      <c r="B68">
-        <v>24532.799999999999</v>
-      </c>
-      <c r="C68">
-        <v>36.630000000000003</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" s="2">
-        <v>45761.791666666657</v>
-      </c>
-      <c r="B69">
-        <v>24587.200000000001</v>
-      </c>
-      <c r="C69">
-        <v>47.02</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" s="2">
-        <v>45761.833333333343</v>
-      </c>
-      <c r="B70">
-        <v>23119.200000000001</v>
-      </c>
-      <c r="C70">
-        <v>37.81</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" s="2">
-        <v>45761.875</v>
-      </c>
-      <c r="B71">
-        <v>22953.200000000001</v>
-      </c>
-      <c r="C71">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" s="2">
-        <v>45761.916666666657</v>
-      </c>
-      <c r="B72">
-        <v>20995</v>
-      </c>
-      <c r="C72">
-        <v>19.75</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" s="2">
-        <v>45761.958333333343</v>
-      </c>
-      <c r="B73">
-        <v>19951.8</v>
-      </c>
-      <c r="C73">
-        <v>13</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
set auto report DA auction FR.
</commit_message>
<xml_diff>
--- a/Data/DA_PriceFR.xlsx
+++ b/Data/DA_PriceFR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CYTech Student\PycharmProjects\Quantitative_Finance\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B029D3C-51F4-4B79-9ED3-F15847C23A07}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49338018-43E9-4909-8C6D-C3744E1D612A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -92,7 +92,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -395,10 +395,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C49"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -419,186 +419,186 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
-        <v>45759</v>
+        <v>45762</v>
       </c>
       <c r="B2">
-        <v>24509.200000000001</v>
+        <v>23237</v>
       </c>
       <c r="C2">
-        <v>34.99</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
-        <v>45759.041666666657</v>
+        <v>45762.041666666657</v>
       </c>
       <c r="B3">
-        <v>24044.6</v>
+        <v>22269</v>
       </c>
       <c r="C3">
-        <v>35</v>
+        <v>7.5</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
-        <v>45759.083333333343</v>
+        <v>45762.083333333343</v>
       </c>
       <c r="B4">
-        <v>24931</v>
+        <v>22199</v>
       </c>
       <c r="C4">
-        <v>31.3</v>
+        <v>5.64</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
-        <v>45759.125</v>
+        <v>45762.125</v>
       </c>
       <c r="B5">
-        <v>25607.200000000001</v>
+        <v>22878</v>
       </c>
       <c r="C5">
-        <v>20.079999999999998</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <v>45759.166666666657</v>
+        <v>45762.166666666657</v>
       </c>
       <c r="B6">
-        <v>25743</v>
+        <v>23060.6</v>
       </c>
       <c r="C6">
-        <v>15.31</v>
+        <v>3.6</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
-        <v>45759.208333333343</v>
+        <v>45762.208333333343</v>
       </c>
       <c r="B7">
-        <v>24152.400000000001</v>
+        <v>21410</v>
       </c>
       <c r="C7">
-        <v>14.99</v>
+        <v>7.08</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
-        <v>45759.25</v>
+        <v>45762.25</v>
       </c>
       <c r="B8">
-        <v>23094.799999999999</v>
+        <v>23536.400000000001</v>
       </c>
       <c r="C8">
-        <v>21.63</v>
+        <v>36.42</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
-        <v>45759.291666666657</v>
+        <v>45762.291666666657</v>
       </c>
       <c r="B9">
-        <v>22935.599999999999</v>
+        <v>25111.4</v>
       </c>
       <c r="C9">
-        <v>27.75</v>
+        <v>34.450000000000003</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
-        <v>45759.333333333343</v>
+        <v>45762.333333333343</v>
       </c>
       <c r="B10">
-        <v>21012.400000000001</v>
+        <v>26717.8</v>
       </c>
       <c r="C10">
-        <v>17.23</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
-        <v>45759.375</v>
+        <v>45762.375</v>
       </c>
       <c r="B11">
-        <v>24349.8</v>
+        <v>29303.200000000001</v>
       </c>
       <c r="C11">
-        <v>8.43</v>
+        <v>48.47</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
-        <v>45759.416666666657</v>
+        <v>45762.416666666657</v>
       </c>
       <c r="B12">
-        <v>27553.8</v>
+        <v>33753.599999999999</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>41.61</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
-        <v>45759.458333333343</v>
+        <v>45762.458333333343</v>
       </c>
       <c r="B13">
-        <v>34918.6</v>
+        <v>37352.6</v>
       </c>
       <c r="C13">
-        <v>-0.02</v>
+        <v>8.5500000000000007</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
-        <v>45759.5</v>
+        <v>45762.5</v>
       </c>
       <c r="B14">
-        <v>39083.800000000003</v>
+        <v>39398</v>
       </c>
       <c r="C14">
-        <v>-7.0000000000000007E-2</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
-        <v>45759.541666666657</v>
+        <v>45762.541666666657</v>
       </c>
       <c r="B15">
-        <v>38749.4</v>
+        <v>40660</v>
       </c>
       <c r="C15">
-        <v>-18.84</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
-        <v>45759.583333333343</v>
+        <v>45762.583333333343</v>
       </c>
       <c r="B16">
-        <v>34564.199999999997</v>
+        <v>41164.800000000003</v>
       </c>
       <c r="C16">
-        <v>-25.38</v>
+        <v>-0.01</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
-        <v>45759.625</v>
+        <v>45762.625</v>
       </c>
       <c r="B17">
-        <v>32419.4</v>
+        <v>42175.6</v>
       </c>
       <c r="C17">
-        <v>-9.93</v>
+        <v>-0.01</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
-        <v>45759.666666666657</v>
+        <v>45762.666666666657</v>
       </c>
       <c r="B18">
-        <v>27329.4</v>
+        <v>42287.199999999997</v>
       </c>
       <c r="C18">
         <v>-0.01</v>
@@ -606,343 +606,79 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
-        <v>45759.708333333343</v>
+        <v>45762.708333333343</v>
       </c>
       <c r="B19">
-        <v>22745.200000000001</v>
+        <v>40936.400000000001</v>
       </c>
       <c r="C19">
-        <v>12.93</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
-        <v>45759.75</v>
+        <v>45762.75</v>
       </c>
       <c r="B20">
-        <v>18975.599999999999</v>
+        <v>39078.800000000003</v>
       </c>
       <c r="C20">
-        <v>32.21</v>
+        <v>11.26</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
-        <v>45759.791666666657</v>
+        <v>45762.791666666657</v>
       </c>
       <c r="B21">
-        <v>20501.8</v>
+        <v>35224.400000000001</v>
       </c>
       <c r="C21">
-        <v>31.62</v>
+        <v>23.5</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
-        <v>45759.833333333343</v>
+        <v>45762.833333333343</v>
       </c>
       <c r="B22">
-        <v>22544.6</v>
+        <v>31807</v>
       </c>
       <c r="C22">
-        <v>44.91</v>
+        <v>33.47</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
-        <v>45759.875</v>
+        <v>45762.875</v>
       </c>
       <c r="B23">
-        <v>25681.599999999999</v>
+        <v>30888.2</v>
       </c>
       <c r="C23">
-        <v>60.55</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
-        <v>45759.916666666657</v>
+        <v>45762.916666666657</v>
       </c>
       <c r="B24">
-        <v>22497.599999999999</v>
+        <v>29298.2</v>
       </c>
       <c r="C24">
-        <v>59.04</v>
+        <v>21.96</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
-        <v>45759.958333333343</v>
+        <v>45762.958333333343</v>
       </c>
       <c r="B25">
-        <v>20205.400000000001</v>
+        <v>28916.400000000001</v>
       </c>
       <c r="C25">
-        <v>38.5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="2">
-        <v>45760</v>
-      </c>
-      <c r="B26">
-        <v>24509.200000000001</v>
-      </c>
-      <c r="C26">
-        <v>34.99</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="2">
-        <v>45760.041666666657</v>
-      </c>
-      <c r="B27">
-        <v>24044.6</v>
-      </c>
-      <c r="C27">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="2">
-        <v>45760.083333333343</v>
-      </c>
-      <c r="B28">
-        <v>24931</v>
-      </c>
-      <c r="C28">
-        <v>31.3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="2">
-        <v>45760.125</v>
-      </c>
-      <c r="B29">
-        <v>25607.200000000001</v>
-      </c>
-      <c r="C29">
-        <v>20.079999999999998</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="2">
-        <v>45760.166666666657</v>
-      </c>
-      <c r="B30">
-        <v>25743</v>
-      </c>
-      <c r="C30">
-        <v>15.31</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="2">
-        <v>45760.208333333343</v>
-      </c>
-      <c r="B31">
-        <v>24152.400000000001</v>
-      </c>
-      <c r="C31">
-        <v>14.99</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="2">
-        <v>45760.25</v>
-      </c>
-      <c r="B32">
-        <v>23094.799999999999</v>
-      </c>
-      <c r="C32">
-        <v>21.63</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="2">
-        <v>45760.291666666657</v>
-      </c>
-      <c r="B33">
-        <v>22935.599999999999</v>
-      </c>
-      <c r="C33">
-        <v>27.75</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="2">
-        <v>45760.333333333343</v>
-      </c>
-      <c r="B34">
-        <v>21012.400000000001</v>
-      </c>
-      <c r="C34">
-        <v>17.23</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="2">
-        <v>45760.375</v>
-      </c>
-      <c r="B35">
-        <v>24349.8</v>
-      </c>
-      <c r="C35">
-        <v>8.43</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="2">
-        <v>45760.416666666657</v>
-      </c>
-      <c r="B36">
-        <v>27553.8</v>
-      </c>
-      <c r="C36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="2">
-        <v>45760.458333333343</v>
-      </c>
-      <c r="B37">
-        <v>34918.6</v>
-      </c>
-      <c r="C37">
-        <v>-0.02</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="2">
-        <v>45760.5</v>
-      </c>
-      <c r="B38">
-        <v>39083.800000000003</v>
-      </c>
-      <c r="C38">
-        <v>-7.0000000000000007E-2</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="2">
-        <v>45760.541666666657</v>
-      </c>
-      <c r="B39">
-        <v>38749.4</v>
-      </c>
-      <c r="C39">
-        <v>-18.84</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="2">
-        <v>45760.583333333343</v>
-      </c>
-      <c r="B40">
-        <v>34564.199999999997</v>
-      </c>
-      <c r="C40">
-        <v>-25.38</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="2">
-        <v>45760.625</v>
-      </c>
-      <c r="B41">
-        <v>32419.4</v>
-      </c>
-      <c r="C41">
-        <v>-9.93</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="2">
-        <v>45760.666666666657</v>
-      </c>
-      <c r="B42">
-        <v>27329.4</v>
-      </c>
-      <c r="C42">
-        <v>-0.01</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="2">
-        <v>45760.708333333343</v>
-      </c>
-      <c r="B43">
-        <v>22745.200000000001</v>
-      </c>
-      <c r="C43">
-        <v>12.93</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="2">
-        <v>45760.75</v>
-      </c>
-      <c r="B44">
-        <v>18975.599999999999</v>
-      </c>
-      <c r="C44">
-        <v>32.21</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="2">
-        <v>45760.791666666657</v>
-      </c>
-      <c r="B45">
-        <v>20501.8</v>
-      </c>
-      <c r="C45">
-        <v>31.62</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="2">
-        <v>45760.833333333343</v>
-      </c>
-      <c r="B46">
-        <v>22544.6</v>
-      </c>
-      <c r="C46">
-        <v>44.91</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="2">
-        <v>45760.875</v>
-      </c>
-      <c r="B47">
-        <v>25681.599999999999</v>
-      </c>
-      <c r="C47">
-        <v>60.55</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="2">
-        <v>45760.916666666657</v>
-      </c>
-      <c r="B48">
-        <v>22497.599999999999</v>
-      </c>
-      <c r="C48">
-        <v>59.04</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="2">
-        <v>45760.958333333343</v>
-      </c>
-      <c r="B49">
-        <v>20205.400000000001</v>
-      </c>
-      <c r="C49">
-        <v>38.5</v>
+        <v>31.9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>